<commit_message>
Refactored war report logic and improved data consistency: - Added timezone-safe comparison for player join date vs war start - Introduced "—" indicator for players not yet in clan during past wars - Cleaned up datetime parsing in report generator - Removed deprecated fetch_and_preview.py (replaced by fetch_latest_data.py) - Standardized clan tag handling via clean_clan_tag() in utils.py - Normalized report generation to align with main pipeline behavior - Confirmed main.py executes full end-to-end data flow without duplication
</commit_message>
<xml_diff>
--- a/reports/war_report.xlsx
+++ b/reports/war_report.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3cbd8aca0faaa1f5/Documents/^N^N^N^NClash of clans war tracker/reports/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_351134B77BAF60025851B4519FE4F7377AE0BEC7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D895FA9-9C09-4E08-AE22-651E9D0F22F1}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="129">
   <si>
     <t>Player Tag</t>
   </si>
@@ -25,6 +31,9 @@
     <t>War 1</t>
   </si>
   <si>
+    <t>War 2</t>
+  </si>
+  <si>
     <t>#QQL2J8JCJ</t>
   </si>
   <si>
@@ -136,12 +145,6 @@
     <t>#YL800RYL2</t>
   </si>
   <si>
-    <t>#QU20RVCU8</t>
-  </si>
-  <si>
-    <t>#PC9GY800G</t>
-  </si>
-  <si>
     <t>#QYGPCQL08</t>
   </si>
   <si>
@@ -163,6 +166,9 @@
     <t>#G9L0UVYP8</t>
   </si>
   <si>
+    <t>#G20Y8UUP8</t>
+  </si>
+  <si>
     <t>ProTayToe</t>
   </si>
   <si>
@@ -274,12 +280,6 @@
     <t>pov_lag_yt</t>
   </si>
   <si>
-    <t>[ACE] EPIC</t>
-  </si>
-  <si>
-    <t>Shakib</t>
-  </si>
-  <si>
     <t>Ragnar Sr.</t>
   </si>
   <si>
@@ -299,6 +299,9 @@
   </si>
   <si>
     <t>protaytoe</t>
+  </si>
+  <si>
+    <t>Lachinio</t>
   </si>
   <si>
     <t>✔ 
@@ -466,13 +469,16 @@
     <t>✔ ⭐
 ⭐⭐⭐ 100.0% M:+0
 ⭐⭐ 66.0% M:+11</t>
+  </si>
+  <si>
+    <t>—</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -538,13 +544,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -582,7 +596,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -616,6 +630,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -650,9 +665,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -825,17 +841,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C47"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="30.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -845,439 +863,559 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>49</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>94</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>50</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>95</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>96</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>97</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>53</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>98</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>99</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>96</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>96</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>100</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>58</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>101</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
         <v>59</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>96</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s">
         <v>60</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>102</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>61</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>103</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
         <v>62</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>104</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>63</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>105</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
         <v>64</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>106</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
         <v>65</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>107</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
         <v>66</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>108</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
         <v>67</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>109</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
         <v>68</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>110</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
         <v>69</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>96</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>111</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
         <v>71</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>112</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
         <v>72</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>96</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
         <v>73</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>113</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
         <v>74</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>114</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
         <v>75</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>115</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
         <v>76</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>116</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
         <v>77</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>106</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
         <v>78</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>117</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
         <v>79</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>118</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
         <v>80</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>119</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
         <v>81</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>120</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
         <v>82</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>121</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
         <v>83</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>122</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B37" t="s">
         <v>84</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>96</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B38" t="s">
         <v>85</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>96</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
         <v>86</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>123</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
         <v>87</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>106</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
         <v>88</v>
@@ -1285,43 +1423,55 @@
       <c r="C41" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="42" spans="1:3">
+      <c r="D41" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B42" t="s">
         <v>89</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>125</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B43" t="s">
         <v>90</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>126</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B44" t="s">
         <v>91</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>106</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B45" t="s">
         <v>92</v>
@@ -1329,27 +1479,22 @@
       <c r="C45" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="46" spans="1:3">
+      <c r="D45" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B46" t="s">
         <v>93</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" t="s">
-        <v>48</v>
-      </c>
-      <c r="B47" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="1" t="s">
         <v>128</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
live testing has gone on with success for 3 iterations of wars, with actionable insights.
</commit_message>
<xml_diff>
--- a/reports/war_report.xlsx
+++ b/reports/war_report.xlsx
@@ -1,20 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3cbd8aca0faaa1f5/Documents/^N^N^N^NClash of clans war tracker/reports/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_2A6556BC305FA52FB651B4FE276B20C979786661" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C51271CA-0561-4D0D-8863-8BA9B293E89F}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Report!$A$1:$E$47</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="193">
   <si>
     <t>Player Tag</t>
   </si>
@@ -166,6 +175,9 @@
     <t>#QL0PCGG9P</t>
   </si>
   <si>
+    <t>#82JJQUYQV</t>
+  </si>
+  <si>
     <t>ProTayToe</t>
   </si>
   <si>
@@ -299,6 +311,9 @@
   </si>
   <si>
     <t>Mr Meow</t>
+  </si>
+  <si>
+    <t>Panda</t>
   </si>
   <si>
     <t>✔ 
@@ -612,13 +627,169 @@
     <t>✔ ⭐⭐⭐⭐
 ⭐⭐⭐ 100.0% M:+0
 ⭐⭐ 70.0% M:+24</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐
+⭐⭐ 91.0% M:+0
+⭐⭐⭐ 100.0% M:-1</t>
+  </si>
+  <si>
+    <t>✔ 
+⭐ 70.0% M:+0</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐⭐
+⭐⭐ 90.0% M:+0
+⭐⭐ 89.0% M:-6</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐⭐
+⭐⭐ 71.0% M:+0
+⭐⭐ 96.0% M:-1</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐
+⭐⭐ 70.0% M:+0
+⭐⭐ 95.0% M:-9</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐⭐⭐
+⭐⭐ 95.0% M:-1
+⭐⭐⭐ 100.0% M:-2</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐
+⭐⭐ 88.0% M:+0
+⭐⭐⭐ 100.0% M:-19</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐⭐⭐
+⭐⭐ 95.0% M:+0
+⭐⭐⭐ 100.0% M:-2</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐⭐⭐⭐
+⭐⭐⭐ 100.0% M:-1
+⭐⭐⭐ 100.0% M:+2</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐
+⭐⭐⭐ 100.0% M:+0
+⭐⭐ 99.0% M:-1</t>
+  </si>
+  <si>
+    <t>✔ ⭐
+⭐ 74.0% M:-3
+⭐ 93.0% M:-2</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐⭐⭐⭐
+⭐⭐⭐ 100.0% M:-2
+⭐⭐⭐ 100.0% M:-1</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐
+⭐ 61.0% M:+0
+⭐⭐ 53.0% M:-1</t>
+  </si>
+  <si>
+    <t>✔ 
+⭐⭐ 86.0% M:-2
+⭐⭐ 96.0% M:-1</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐⭐⭐
+⭐⭐⭐ 100.0% M:-14
+⭐⭐ 93.0% M:-13</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐⭐⭐
+⭐⭐ 84.0% M:+0
+⭐⭐⭐ 100.0% M:-1</t>
+  </si>
+  <si>
+    <t>✔ 
+⭐ 67.0% M:-6
+⭐⭐ 60.0% M:+5</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐
+⭐⭐ 98.0% M:-12</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐
+⭐⭐ 87.0% M:+0
+⭐⭐ 74.0% M:-5</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐⭐⭐
+⭐⭐⭐ 100.0% M:+0
+⭐⭐ 77.0% M:-1</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐
+⭐⭐ 78.0% M:+0
+⭐⭐ 77.0% M:-12</t>
+  </si>
+  <si>
+    <t>✔ ⭐
+⭐⭐ 62.0% M:+4
+⭐ 40.0% M:+5</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐⭐⭐⭐
+⭐⭐⭐ 100.0% M:-13
+⭐⭐⭐ 100.0% M:+1</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐⭐
+⭐⭐ 69.0% M:+0
+⭐⭐ 62.0% M:-7</t>
+  </si>
+  <si>
+    <t>✔ ⭐
+⭐⭐ 77.0% M:-9
+⭐⭐⭐ 100.0% M:-10</t>
+  </si>
+  <si>
+    <t>✔ 
+⭐⭐ 73.0% M:-11</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐⭐
+⭐⭐⭐ 100.0% M:+0
+⭐⭐ 83.0% M:-2</t>
+  </si>
+  <si>
+    <t>✔ 
+⭐⭐ 90.0% M:+0
+⭐⭐ 69.0% M:-3</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐⭐
+⭐⭐⭐ 100.0% M:-3
+⭐⭐⭐ 100.0% M:-2</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐⭐⭐
+⭐⭐⭐ 100.0% M:+0
+⭐⭐ 69.0% M:+6</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐⭐⭐⭐
+⭐⭐⭐ 100.0% M:+2
+⭐⭐⭐ 100.0% M:+15</t>
+  </si>
+  <si>
+    <t>✔ ⭐⭐⭐
+⭐⭐⭐ 100.0% M:-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -635,12 +806,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -670,7 +847,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -678,19 +855,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -728,7 +917,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -762,6 +951,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -796,9 +986,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -971,17 +1162,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="5" width="30.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -998,772 +1191,790 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
-        <v>67</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="E19" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
       <c r="B29" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="A32" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
-      <c r="A33" t="s">
+      <c r="B32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B33" t="s">
-        <v>81</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="B33" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
       <c r="B37" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>44</v>
       </c>
       <c r="B41" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>45</v>
       </c>
       <c r="B42" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>46</v>
       </c>
       <c r="B43" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
       <c r="B44" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>48</v>
       </c>
       <c r="B45" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E47" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>